<commit_message>
Results to Kathleen - No HR noLOC
</commit_message>
<xml_diff>
--- a/ResultsOutput/indQ_LOC-NO_lhs2_conf50_nosubset_clust.xlsx
+++ b/ResultsOutput/indQ_LOC-NO_lhs2_conf50_nosubset_clust.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/azp271/Library/Mobile Documents/com~apple~CloudDocs/Documents/Research/PSU/CrossStudyDataAnalysis/LOCeating_ARM/ResultsOutput/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A040B0-ED8D-6D42-BD81-2DED8095FBD8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF484A4-E707-F442-BA68-3C865C0C544A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13940" yWindow="1040" windowWidth="27640" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="indQ_LOC-NO_lhs2_conf50_nosubse" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,13 @@
   </definedNames>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId3"/>
+    <pivotCache cacheId="37" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="44">
   <si>
     <t>LHS2</t>
   </si>
@@ -92,15 +92,6 @@
     <t>cebq34_lsSometimes</t>
   </si>
   <si>
-    <t>cebq26_gRarely</t>
-  </si>
-  <si>
-    <t>gR_SR</t>
-  </si>
-  <si>
-    <t>cAge_8.10yr</t>
-  </si>
-  <si>
     <t>cebq1_gRarely</t>
   </si>
   <si>
@@ -119,9 +110,6 @@
     <t>lsS_EOE</t>
   </si>
   <si>
-    <t>mEducation_gHS</t>
-  </si>
-  <si>
     <t>cebq5_gRarely</t>
   </si>
   <si>
@@ -131,21 +119,6 @@
     <t>cebq20_gRarely</t>
   </si>
   <si>
-    <t>cebq21_gRarely</t>
-  </si>
-  <si>
-    <t>lsS_DD</t>
-  </si>
-  <si>
-    <t>cebq31_lsSometimes</t>
-  </si>
-  <si>
-    <t>gN_Rest</t>
-  </si>
-  <si>
-    <t>cfq23_gNeutralAD</t>
-  </si>
-  <si>
     <t>Column Labels</t>
   </si>
   <si>
@@ -173,7 +146,19 @@
     <t>kappa</t>
   </si>
   <si>
-    <t>Cluster_gupta3</t>
+    <t>OR_upperCI</t>
+  </si>
+  <si>
+    <t>Cluster_gupta2</t>
+  </si>
+  <si>
+    <t>(Multiple Items)</t>
+  </si>
+  <si>
+    <t>gR_EF Total</t>
+  </si>
+  <si>
+    <t>gR_SE Total</t>
   </si>
 </sst>
 </file>
@@ -657,15 +642,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -726,7 +708,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Alaina Pearce" refreshedDate="43997.564218749998" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="17" xr:uid="{00000000-000A-0000-FFFF-FFFF1E000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Alaina Pearce" refreshedDate="43998.767714699075" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="12" xr:uid="{00000000-000A-0000-FFFF-FFFF1E000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:Q1048576" sheet="indQ_LOC-NO_lhs2_conf50_nosubse"/>
   </cacheSource>
@@ -735,7 +717,6 @@
       <sharedItems containsBlank="1" count="57">
         <m/>
         <s v="cebq34_lsSometimes"/>
-        <s v="cfq23_gNeutralAD"/>
         <s v="cebq7_gRarely" u="1"/>
         <s v="cebq5_gRarely" u="1"/>
         <s v="cebq1_gRarely" u="1"/>
@@ -753,6 +734,7 @@
         <s v="cebq11_gRarely" u="1"/>
         <s v="mEducation_gHS" u="1"/>
         <s v="cebq22=Often" u="1"/>
+        <s v="cfq23_gNeutralAD" u="1"/>
         <s v="cfq24_gNeutralAD" u="1"/>
         <s v="cebq19=Rarely" u="1"/>
         <s v="cebq1_gSometimes" u="1"/>
@@ -795,21 +777,16 @@
     <cacheField name="LHS1" numFmtId="0">
       <sharedItems containsBlank="1" count="74">
         <s v="cebq34_lsSometimes"/>
-        <s v="cAge_8.10yr"/>
         <s v="cBMI=HW"/>
-        <s v="cebq13_lsSometimes"/>
+        <s v="cebq1_gRarely"/>
         <s v="cebq14_lsSometimes"/>
         <s v="cebq15_lsSometimes"/>
-        <s v="cebq1_gRarely"/>
-        <s v="cebq21_gRarely"/>
+        <s v="cebq20_gRarely"/>
+        <s v="cebq13_lsSometimes"/>
+        <s v="cebq5_gRarely"/>
         <s v="cebq8_gRarely"/>
-        <s v="cebq31_lsSometimes"/>
-        <s v="cebq20_gRarely"/>
-        <s v="cebq5_gRarely"/>
         <s v="income_g50K"/>
         <s v="income_g75K"/>
-        <s v="mEducation_gHS"/>
-        <s v="cebq26_gRarely"/>
         <m/>
         <s v="cebq9_gRarely" u="1"/>
         <s v="cebq7_gRarely" u="1"/>
@@ -824,9 +801,11 @@
         <s v="cAge_8.9yr" u="1"/>
         <s v="cfq9=Avg" u="1"/>
         <s v="sex=Female" u="1"/>
+        <s v="cebq26_gRarely" u="1"/>
         <s v="cebq3_gRarelyRev" u="1"/>
         <s v="cebq4_gRarelyRev" u="1"/>
         <s v="cebq11_gRarely" u="1"/>
+        <s v="mEducation_gHS" u="1"/>
         <s v="cebq19=Rarely" u="1"/>
         <s v="cebq10=Sometimes" u="1"/>
         <s v="cebq17=Sometimes" u="1"/>
@@ -859,13 +838,16 @@
         <s v="cebq9_lsSometimes" u="1"/>
         <s v="cfq6=Avg" u="1"/>
         <s v="cebq8=Sometimes" u="1"/>
+        <s v="cebq21_gRarely" u="1"/>
         <s v="cebq34=Rarely" u="1"/>
         <s v="cebq29=Rarely" u="1"/>
         <s v="cebq14=Rarely" u="1"/>
+        <s v="cAge_8.10yr" u="1"/>
         <s v="cebq19_lsSometimes" u="1"/>
         <s v="cebq24_lsSometimes" u="1"/>
         <s v="cebq27_lsSometimes" u="1"/>
         <s v="cebq29_lsSometimes" u="1"/>
+        <s v="cebq31_lsSometimes" u="1"/>
         <s v="cebq33_lsSometimes" u="1"/>
         <s v="cebq2=Rarely" u="1"/>
       </sharedItems>
@@ -873,59 +855,64 @@
     <cacheField name="RHS" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
-    <cacheField name="lift" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.0828462003628301" maxValue="1.19875355642867"/>
+    <cacheField name="count" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="61" maxValue="102"/>
     </cacheField>
     <cacheField name="support" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.354430379746835" maxValue="0.645569620253165"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.386075949367089" maxValue="0.645569620253165"/>
     </cacheField>
     <cacheField name="confidence" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.82926829268292701" maxValue="0.91803278688524603"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.82926829268292701" maxValue="0.89705882352941202"/>
     </cacheField>
     <cacheField name="coverage" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.386075949367089" maxValue="0.778481012658228"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.430379746835443" maxValue="0.778481012658228"/>
     </cacheField>
-    <cacheField name="count" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="56" maxValue="102"/>
+    <cacheField name="lift" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.0828462003628301" maxValue="1.17136606708799"/>
+    </cacheField>
+    <cacheField name="addVal" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="6.3445507872800205E-2" maxValue="0.13123603871928499"/>
+    </cacheField>
+    <cacheField name="kappa" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.210353573027003" maxValue="0.28067379922604102"/>
     </cacheField>
     <cacheField name="oddsRatio" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="2.8617886178861802" maxValue="5.5138461538461501"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="3.1466165413533802" maxValue="4.3571428571428603"/>
     </cacheField>
-    <cacheField name="addVal" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="6.3445507872800205E-2" maxValue="0.15221000207511901"/>
+    <cacheField name="OR_lowerCI" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.45577217627033" maxValue="1.81198382412186"/>
+    </cacheField>
+    <cacheField name="OR_upperCI" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="6.8013359643165403" maxValue="10.680261187261699"/>
+    </cacheField>
+    <cacheField name="fisher.p" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="4.9535558537442802E-4" maxValue="3.3158310083905101E-3"/>
     </cacheField>
     <cacheField name="fisher.padj_holm" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="3.0000000000000001E-3" maxValue="1.32E-2"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5.4000000000000003E-3" maxValue="6.0000000000000001E-3"/>
     </cacheField>
-    <cacheField name="OR_lowerCI" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.34292165572156" maxValue="2.0122604092032601"/>
-    </cacheField>
-    <cacheField name="kappa" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.20448270261491" maxValue="0.28067379922604102"/>
-    </cacheField>
-    <cacheField name="fisher.p" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.8980410385483401E-4" maxValue="5.0826707024197396E-3"/>
-    </cacheField>
-    <cacheField name="Cluster_gupta3" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="3"/>
+    <cacheField name="Cluster_gupta2" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="2" count="3">
+        <n v="2"/>
+        <n v="1"/>
+        <m/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Cat1" numFmtId="0">
       <sharedItems containsBlank="1" count="42">
         <s v="lsS_FR"/>
-        <s v="cAge_8.10yr"/>
         <s v="cBMI=HW"/>
+        <s v="gR_EF"/>
         <s v="lsS_EOE"/>
-        <s v="gR_EF"/>
-        <s v="gR_SR"/>
         <s v="gR_SE"/>
-        <s v="lsS_DD"/>
         <s v="income_g50K"/>
         <s v="income_g75K"/>
-        <s v="mEducation_gHS"/>
         <m/>
+        <s v="cAge_8.10yr" u="1"/>
         <s v="dBMI_OBOW" u="1"/>
         <s v="cAge_9.10yr" u="1"/>
         <s v="BreastFed_least4mo" u="1"/>
+        <s v="mEducation_gHS" u="1"/>
         <s v="PPW_UW" u="1"/>
         <s v="mEducation_gAssoc" u="1"/>
         <s v="lsS_EUE" u="1"/>
@@ -943,56 +930,18 @@
         <s v="Female" u="1"/>
         <s v="lsS_FF" u="1"/>
         <s v="sFF" u="1"/>
+        <s v="gR_SR" u="1"/>
         <s v="lsDD" u="1"/>
         <s v="sSR" u="1"/>
         <s v="sEUE" u="1"/>
         <s v="gMon" u="1"/>
         <s v="gR_FF" u="1"/>
+        <s v="lsS_DD" u="1"/>
         <s v="Male" u="1"/>
         <s v="gR_FR" u="1"/>
         <s v="cAge_8.9yr" u="1"/>
         <s v="lsEOE" u="1"/>
         <s v="gEF" u="1"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Cat2" numFmtId="0">
-      <sharedItems containsBlank="1" count="36">
-        <s v="NA"/>
-        <s v="lsS_FR"/>
-        <s v="gN_Rest"/>
-        <m/>
-        <s v="mEducation_gHS" u="1"/>
-        <s v="PPW_UW" u="1"/>
-        <s v="income_g50K" u="1"/>
-        <s v="gR_DD" u="1"/>
-        <s v="PPW_avg" u="1"/>
-        <s v="cBMI=HW" u="1"/>
-        <s v="sSE" u="1"/>
-        <s v="lsFR" u="1"/>
-        <s v="gS_EF" u="1"/>
-        <s v="BreastFed_ls10mo" u="1"/>
-        <s v="gS_FR" u="1"/>
-        <s v="PCW_UW" u="1"/>
-        <s v="gS_PR" u="1"/>
-        <s v="mBMI=HealthyWeight" u="1"/>
-        <s v="gR_EUE" u="1"/>
-        <s v="lsS_FF" u="1"/>
-        <s v="sFF" u="1"/>
-        <s v="gR_SR" u="1"/>
-        <s v="gR_SE" u="1"/>
-        <s v="lsDD" u="1"/>
-        <s v="sSR" u="1"/>
-        <s v="sEUE" u="1"/>
-        <s v="gR_FF" u="1"/>
-        <s v="lsS_DD" u="1"/>
-        <s v="lsN_PE" u="1"/>
-        <s v="gR_EF" u="1"/>
-        <s v="gR_FR" u="1"/>
-        <s v="EatFamily_g1wk" u="1"/>
-        <s v="lsEOE" u="1"/>
-        <s v="gEF" u="1"/>
-        <s v="lsS_EOE" u="1"/>
-        <s v="income_g75K" u="1"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -1005,23 +954,23 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="17">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="12">
   <r>
     <x v="0"/>
     <x v="0"/>
     <s v="loc1=No"/>
-    <n v="1.0828462003628301"/>
+    <n v="102"/>
     <n v="0.645569620253165"/>
     <n v="0.82926829268292701"/>
     <n v="0.778481012658228"/>
-    <n v="102"/>
+    <n v="1.0828462003628301"/>
+    <n v="6.3445507872800205E-2"/>
+    <n v="0.28067379922604102"/>
     <n v="4.0902255639097698"/>
-    <n v="6.3445507872800205E-2"/>
-    <n v="9.1000000000000004E-3"/>
     <n v="1.81198382412186"/>
-    <n v="0.28067379922604102"/>
+    <n v="9.2329439926258097"/>
     <n v="7.7238946177791404E-4"/>
-    <n v="3"/>
+    <n v="6.0000000000000001E-3"/>
     <x v="0"/>
     <x v="0"/>
   </r>
@@ -1029,290 +978,195 @@
     <x v="1"/>
     <x v="1"/>
     <s v="loc1=No"/>
-    <n v="1.12143898881867"/>
-    <n v="0.462025316455696"/>
-    <n v="0.85882352941176499"/>
-    <n v="0.537974683544304"/>
-    <n v="73"/>
-    <n v="3.1684027777777799"/>
-    <n v="9.3000744601638097E-2"/>
-    <n v="1.32E-2"/>
-    <n v="1.45422802106559"/>
-    <n v="0.208549006511939"/>
-    <n v="2.56285631828944E-3"/>
-    <n v="3"/>
-    <x v="1"/>
+    <n v="80"/>
+    <n v="0.506329113924051"/>
+    <n v="0.85106382978723405"/>
+    <n v="0.59493670886076"/>
+    <n v="1.1113064884824999"/>
+    <n v="8.5241044977107494E-2"/>
+    <n v="0.225628230261985"/>
+    <n v="3.2055749128919899"/>
+    <n v="1.4936951655941699"/>
+    <n v="6.8793892882922503"/>
+    <n v="2.1365073142274099E-3"/>
+    <n v="6.0000000000000001E-3"/>
+    <x v="0"/>
     <x v="1"/>
   </r>
   <r>
     <x v="1"/>
     <x v="2"/>
     <s v="loc1=No"/>
-    <n v="1.1113064884824999"/>
-    <n v="0.506329113924051"/>
-    <n v="0.85106382978723405"/>
-    <n v="0.59493670886076"/>
-    <n v="80"/>
-    <n v="3.2055749128919899"/>
-    <n v="8.5241044977107494E-2"/>
-    <n v="1.32E-2"/>
-    <n v="1.4936951655941699"/>
-    <n v="0.225628230261985"/>
-    <n v="2.1365073142274099E-3"/>
-    <n v="3"/>
+    <n v="99"/>
+    <n v="0.626582278481013"/>
+    <n v="0.83193277310924396"/>
+    <n v="0.753164556962025"/>
+    <n v="1.08632543926662"/>
+    <n v="6.6109988299117198E-2"/>
+    <n v="0.272527954395966"/>
+    <n v="3.8250000000000002"/>
+    <n v="1.72789193530244"/>
+    <n v="8.4673263999227899"/>
+    <n v="9.8327872889956893E-4"/>
+    <n v="6.0000000000000001E-3"/>
+    <x v="0"/>
     <x v="2"/>
-    <x v="1"/>
   </r>
   <r>
     <x v="1"/>
     <x v="3"/>
     <s v="loc1=No"/>
-    <n v="1.09211119459053"/>
-    <n v="0.582278481012658"/>
-    <n v="0.83636363636363598"/>
-    <n v="0.69620253164557"/>
-    <n v="92"/>
-    <n v="3.3486590038314201"/>
-    <n v="7.0540851553509795E-2"/>
-    <n v="1.32E-2"/>
-    <n v="1.5535635949761399"/>
-    <n v="0.24822838631301899"/>
-    <n v="1.8891248571212499E-3"/>
-    <n v="3"/>
-    <x v="3"/>
-    <x v="1"/>
+    <n v="67"/>
+    <n v="0.424050632911392"/>
+    <n v="0.88157894736842102"/>
+    <n v="0.481012658227848"/>
+    <n v="1.1511526750761201"/>
+    <n v="0.115756162558294"/>
+    <n v="0.21831317732055899"/>
+    <n v="3.8600823045267498"/>
+    <n v="1.6795218483229"/>
+    <n v="8.8717127512210006"/>
+    <n v="7.5582914448785198E-4"/>
+    <n v="6.0000000000000001E-3"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
     <x v="4"/>
     <s v="loc1=No"/>
-    <n v="1.1511526750761201"/>
-    <n v="0.424050632911392"/>
-    <n v="0.88157894736842102"/>
-    <n v="0.481012658227848"/>
-    <n v="67"/>
-    <n v="3.8600823045267498"/>
-    <n v="0.115756162558294"/>
-    <n v="9.1000000000000004E-3"/>
-    <n v="1.6795218483229"/>
-    <n v="0.21831317732055899"/>
-    <n v="7.5582914448785198E-4"/>
-    <n v="3"/>
+    <n v="93"/>
+    <n v="0.588607594936709"/>
+    <n v="0.83035714285714302"/>
+    <n v="0.708860759493671"/>
+    <n v="1.0842680047225499"/>
+    <n v="6.4534358047016294E-2"/>
+    <n v="0.235221421215242"/>
+    <n v="3.1466165413533802"/>
+    <n v="1.45577217627033"/>
+    <n v="6.8013359643165403"/>
+    <n v="3.3158310083905101E-3"/>
+    <n v="6.0000000000000001E-3"/>
     <x v="0"/>
-    <x v="1"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="1"/>
     <x v="5"/>
     <s v="loc1=No"/>
-    <n v="1.0842680047225499"/>
+    <n v="93"/>
     <n v="0.588607594936709"/>
-    <n v="0.83035714285714302"/>
-    <n v="0.708860759493671"/>
-    <n v="93"/>
-    <n v="3.1466165413533802"/>
-    <n v="6.4534358047016294E-2"/>
-    <n v="1.32E-2"/>
-    <n v="1.45577217627033"/>
-    <n v="0.235221421215242"/>
-    <n v="3.3158310083905101E-3"/>
-    <n v="3"/>
-    <x v="3"/>
-    <x v="1"/>
+    <n v="0.83783783783783805"/>
+    <n v="0.70253164556962"/>
+    <n v="1.09403618494528"/>
+    <n v="7.2015053027711301E-2"/>
+    <n v="0.25791300796406003"/>
+    <n v="3.50595238095238"/>
+    <n v="1.6220177643011999"/>
+    <n v="7.5780317380193498"/>
+    <n v="1.3413825557096299E-3"/>
+    <n v="6.0000000000000001E-3"/>
+    <x v="0"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="1"/>
     <x v="6"/>
     <s v="loc1=No"/>
-    <n v="1.08632543926662"/>
-    <n v="0.626582278481013"/>
-    <n v="0.83193277310924396"/>
-    <n v="0.753164556962025"/>
-    <n v="99"/>
-    <n v="3.8250000000000002"/>
-    <n v="6.6109988299117198E-2"/>
-    <n v="9.1000000000000004E-3"/>
-    <n v="1.72789193530244"/>
-    <n v="0.272527954395966"/>
-    <n v="9.8327872889956893E-4"/>
-    <n v="3"/>
-    <x v="4"/>
-    <x v="1"/>
+    <n v="92"/>
+    <n v="0.582278481012658"/>
+    <n v="0.83636363636363598"/>
+    <n v="0.69620253164557"/>
+    <n v="1.09211119459053"/>
+    <n v="7.0540851553509795E-2"/>
+    <n v="0.24822838631301899"/>
+    <n v="3.3486590038314201"/>
+    <n v="1.5535635949761399"/>
+    <n v="7.21793247486172"/>
+    <n v="1.8891248571212499E-3"/>
+    <n v="6.0000000000000001E-3"/>
+    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="1"/>
     <x v="7"/>
     <s v="loc1=No"/>
-    <n v="1.1070786920589299"/>
-    <n v="0.493670886075949"/>
-    <n v="0.84782608695652195"/>
-    <n v="0.582278481012658"/>
-    <n v="78"/>
-    <n v="2.9800664451827199"/>
-    <n v="8.2003302146395202E-2"/>
-    <n v="1.32E-2"/>
-    <n v="1.3914650555213"/>
-    <n v="0.209306409130816"/>
-    <n v="3.7727982342369501E-3"/>
-    <n v="3"/>
-    <x v="5"/>
-    <x v="1"/>
+    <n v="97"/>
+    <n v="0.613924050632911"/>
+    <n v="0.83620689655172398"/>
+    <n v="0.734177215189874"/>
+    <n v="1.0919065260758001"/>
+    <n v="7.0384111741597505E-2"/>
+    <n v="0.27522935779816499"/>
+    <n v="3.82894736842105"/>
+    <n v="1.74750749450523"/>
+    <n v="8.3895708580576898"/>
+    <n v="8.0570904900294997E-4"/>
+    <n v="6.0000000000000001E-3"/>
+    <x v="0"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="1"/>
     <x v="8"/>
     <s v="loc1=No"/>
-    <n v="1.1251978195885399"/>
+    <n v="81"/>
     <n v="0.512658227848101"/>
     <n v="0.86170212765957399"/>
     <n v="0.594936708860759"/>
-    <n v="81"/>
+    <n v="1.1251978195885399"/>
+    <n v="9.5879342849447893E-2"/>
+    <n v="0.25378720370700403"/>
     <n v="3.7384615384615398"/>
-    <n v="9.5879342849447893E-2"/>
-    <n v="7.7999999999999996E-3"/>
     <n v="1.7240849535192999"/>
-    <n v="0.25378720370700403"/>
+    <n v="8.1063839957697095"/>
     <n v="5.9937858995312804E-4"/>
-    <n v="3"/>
-    <x v="6"/>
-    <x v="1"/>
+    <n v="5.4000000000000003E-3"/>
+    <x v="0"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="1"/>
     <x v="9"/>
     <s v="loc1=No"/>
-    <n v="1.1284562799714299"/>
-    <n v="0.443037974683544"/>
-    <n v="0.86419753086419704"/>
-    <n v="0.512658227848101"/>
-    <n v="70"/>
-    <n v="3.24420677361854"/>
-    <n v="9.83747460540709E-2"/>
-    <n v="1.32E-2"/>
-    <n v="1.4694879318405401"/>
-    <n v="0.20448270261491"/>
-    <n v="2.3400287404868598E-3"/>
-    <n v="3"/>
-    <x v="7"/>
+    <n v="61"/>
+    <n v="0.386075949367089"/>
+    <n v="0.89705882352941202"/>
+    <n v="0.430379746835443"/>
+    <n v="1.17136606708799"/>
+    <n v="0.13123603871928499"/>
+    <n v="0.210353573027003"/>
+    <n v="4.3571428571428603"/>
+    <n v="1.77754958841213"/>
+    <n v="10.680261187261699"/>
+    <n v="4.9535558537442802E-4"/>
+    <n v="5.4000000000000003E-3"/>
     <x v="1"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="1"/>
     <x v="10"/>
     <s v="loc1=No"/>
-    <n v="1.09403618494528"/>
-    <n v="0.588607594936709"/>
-    <n v="0.83783783783783805"/>
-    <n v="0.70253164556962"/>
-    <n v="93"/>
-    <n v="3.50595238095238"/>
-    <n v="7.2015053027711301E-2"/>
-    <n v="1.0699999999999999E-2"/>
-    <n v="1.6220177643011999"/>
-    <n v="0.25791300796406003"/>
-    <n v="1.3413825557096299E-3"/>
-    <n v="3"/>
-    <x v="4"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="11"/>
-    <s v="loc1=No"/>
-    <n v="1.0919065260758001"/>
-    <n v="0.613924050632911"/>
-    <n v="0.83620689655172398"/>
-    <n v="0.734177215189874"/>
-    <n v="97"/>
-    <n v="3.82894736842105"/>
-    <n v="7.0384111741597505E-2"/>
-    <n v="9.1000000000000004E-3"/>
-    <n v="1.74750749450523"/>
-    <n v="0.27522935779816499"/>
-    <n v="8.0570904900294997E-4"/>
-    <n v="3"/>
-    <x v="4"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="12"/>
-    <s v="loc1=No"/>
-    <n v="1.17136606708799"/>
+    <n v="61"/>
     <n v="0.386075949367089"/>
     <n v="0.89705882352941202"/>
     <n v="0.430379746835443"/>
-    <n v="61"/>
+    <n v="1.17136606708799"/>
+    <n v="0.13123603871928499"/>
+    <n v="0.210353573027003"/>
     <n v="4.3571428571428603"/>
-    <n v="0.13123603871928499"/>
-    <n v="7.4000000000000003E-3"/>
     <n v="1.77754958841213"/>
-    <n v="0.210353573027003"/>
+    <n v="10.680261187261699"/>
     <n v="4.9535558537442802E-4"/>
-    <n v="2"/>
-    <x v="8"/>
+    <n v="5.4000000000000003E-3"/>
     <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="13"/>
-    <s v="loc1=No"/>
-    <n v="1.17136606708799"/>
-    <n v="0.386075949367089"/>
-    <n v="0.89705882352941202"/>
-    <n v="0.430379746835443"/>
-    <n v="61"/>
-    <n v="4.3571428571428603"/>
-    <n v="0.13123603871928499"/>
-    <n v="7.4000000000000003E-3"/>
-    <n v="1.77754958841213"/>
-    <n v="0.210353573027003"/>
-    <n v="4.9535558537442802E-4"/>
-    <n v="2"/>
-    <x v="9"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="14"/>
-    <s v="loc1=No"/>
-    <n v="1.0996085254458501"/>
-    <n v="0.506329113924051"/>
-    <n v="0.84210526315789502"/>
-    <n v="0.60126582278481"/>
-    <n v="80"/>
-    <n v="2.8617886178861802"/>
-    <n v="7.6282478347768107E-2"/>
-    <n v="1.32E-2"/>
-    <n v="1.34292165572156"/>
-    <n v="0.205602442090142"/>
-    <n v="5.0826707024197396E-3"/>
-    <n v="3"/>
-    <x v="10"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="15"/>
-    <s v="loc1=No"/>
-    <n v="1.19875355642867"/>
-    <n v="0.354430379746835"/>
-    <n v="0.91803278688524603"/>
-    <n v="0.386075949367089"/>
-    <n v="56"/>
-    <n v="5.5138461538461501"/>
-    <n v="0.15221000207511901"/>
-    <n v="3.0000000000000001E-3"/>
-    <n v="2.0122604092032601"/>
-    <n v="0.20966128340717399"/>
-    <n v="1.8980410385483401E-4"/>
-    <n v="1"/>
-    <x v="5"/>
-    <x v="2"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="0"/>
-    <x v="16"/>
+    <x v="11"/>
     <m/>
     <m/>
     <m/>
@@ -1326,23 +1180,23 @@
     <m/>
     <m/>
     <m/>
-    <x v="11"/>
-    <x v="3"/>
+    <x v="2"/>
+    <x v="7"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable5" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:O11" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable5" cacheId="37" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:M8" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="17">
     <pivotField axis="axisRow" showAll="0">
       <items count="58">
         <item m="1" x="31"/>
-        <item m="1" x="8"/>
-        <item m="1" x="5"/>
+        <item m="1" x="7"/>
+        <item m="1" x="4"/>
         <item m="1" x="22"/>
-        <item m="1" x="17"/>
+        <item m="1" x="16"/>
         <item m="1" x="50"/>
         <item m="1" x="51"/>
         <item m="1" x="48"/>
@@ -1352,20 +1206,20 @@
         <item m="1" x="53"/>
         <item m="1" x="21"/>
         <item m="1" x="40"/>
-        <item m="1" x="7"/>
+        <item m="1" x="6"/>
         <item m="1" x="43"/>
         <item m="1" x="38"/>
-        <item m="1" x="19"/>
-        <item m="1" x="10"/>
+        <item m="1" x="18"/>
+        <item m="1" x="9"/>
         <item m="1" x="23"/>
         <item m="1" x="33"/>
-        <item m="1" x="14"/>
+        <item m="1" x="13"/>
         <item m="1" x="24"/>
         <item m="1" x="35"/>
         <item m="1" x="39"/>
         <item m="1" x="54"/>
         <item m="1" x="47"/>
-        <item m="1" x="15"/>
+        <item m="1" x="14"/>
         <item m="1" x="32"/>
         <item m="1" x="55"/>
         <item m="1" x="36"/>
@@ -1373,107 +1227,107 @@
         <item m="1" x="56"/>
         <item x="1"/>
         <item m="1" x="46"/>
-        <item m="1" x="6"/>
-        <item m="1" x="16"/>
-        <item m="1" x="4"/>
+        <item m="1" x="5"/>
+        <item m="1" x="15"/>
+        <item m="1" x="3"/>
         <item m="1" x="27"/>
-        <item m="1" x="3"/>
-        <item m="1" x="12"/>
+        <item m="1" x="2"/>
+        <item m="1" x="11"/>
         <item m="1" x="26"/>
         <item m="1" x="42"/>
-        <item m="1" x="9"/>
+        <item m="1" x="8"/>
         <item m="1" x="29"/>
-        <item x="2"/>
+        <item m="1" x="19"/>
         <item m="1" x="20"/>
-        <item m="1" x="11"/>
+        <item m="1" x="10"/>
         <item m="1" x="34"/>
         <item m="1" x="41"/>
-        <item m="1" x="13"/>
+        <item m="1" x="12"/>
         <item m="1" x="45"/>
         <item m="1" x="44"/>
         <item m="1" x="37"/>
         <item m="1" x="49"/>
-        <item m="1" x="18"/>
+        <item m="1" x="17"/>
         <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisCol" showAll="0">
       <items count="75">
+        <item m="1" x="49"/>
+        <item m="1" x="45"/>
+        <item m="1" x="66"/>
+        <item m="1" x="22"/>
+        <item m="1" x="44"/>
+        <item m="1" x="42"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item m="1" x="31"/>
+        <item m="1" x="28"/>
+        <item x="6"/>
+        <item m="1" x="17"/>
+        <item x="3"/>
+        <item m="1" x="65"/>
+        <item x="4"/>
+        <item m="1" x="43"/>
+        <item m="1" x="41"/>
+        <item m="1" x="32"/>
+        <item m="1" x="19"/>
+        <item m="1" x="67"/>
+        <item m="1" x="30"/>
+        <item m="1" x="57"/>
+        <item m="1" x="73"/>
+        <item x="5"/>
+        <item m="1" x="54"/>
+        <item m="1" x="62"/>
+        <item m="1" x="33"/>
+        <item m="1" x="55"/>
+        <item m="1" x="18"/>
+        <item m="1" x="34"/>
+        <item m="1" x="68"/>
+        <item m="1" x="47"/>
+        <item m="1" x="25"/>
+        <item m="1" x="35"/>
+        <item m="1" x="69"/>
+        <item m="1" x="51"/>
+        <item m="1" x="56"/>
+        <item m="1" x="70"/>
+        <item m="1" x="64"/>
+        <item m="1" x="26"/>
+        <item m="1" x="46"/>
+        <item m="1" x="36"/>
+        <item m="1" x="71"/>
         <item m="1" x="52"/>
+        <item m="1" x="72"/>
+        <item m="1" x="37"/>
+        <item x="0"/>
+        <item m="1" x="63"/>
+        <item m="1" x="27"/>
+        <item x="7"/>
+        <item m="1" x="38"/>
+        <item m="1" x="14"/>
+        <item m="1" x="40"/>
+        <item m="1" x="58"/>
+        <item m="1" x="13"/>
+        <item m="1" x="21"/>
+        <item x="8"/>
+        <item m="1" x="61"/>
+        <item m="1" x="12"/>
+        <item m="1" x="59"/>
+        <item m="1" x="39"/>
+        <item m="1" x="50"/>
+        <item m="1" x="60"/>
+        <item m="1" x="15"/>
+        <item m="1" x="23"/>
+        <item m="1" x="53"/>
         <item m="1" x="48"/>
-        <item x="1"/>
-        <item m="1" x="27"/>
-        <item m="1" x="47"/>
-        <item m="1" x="45"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item m="1" x="34"/>
-        <item m="1" x="32"/>
-        <item x="3"/>
-        <item m="1" x="22"/>
-        <item x="4"/>
-        <item m="1" x="67"/>
-        <item x="5"/>
-        <item m="1" x="46"/>
-        <item m="1" x="44"/>
-        <item m="1" x="35"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item m="1" x="20"/>
+        <item m="1" x="29"/>
         <item m="1" x="24"/>
-        <item m="1" x="68"/>
-        <item m="1" x="33"/>
-        <item m="1" x="60"/>
-        <item m="1" x="73"/>
-        <item x="10"/>
-        <item m="1" x="57"/>
-        <item x="7"/>
-        <item m="1" x="36"/>
-        <item m="1" x="58"/>
-        <item m="1" x="23"/>
-        <item m="1" x="37"/>
-        <item m="1" x="69"/>
-        <item m="1" x="50"/>
-        <item x="15"/>
-        <item m="1" x="38"/>
-        <item m="1" x="70"/>
-        <item m="1" x="54"/>
-        <item m="1" x="59"/>
-        <item m="1" x="71"/>
-        <item m="1" x="66"/>
-        <item m="1" x="30"/>
-        <item m="1" x="49"/>
-        <item m="1" x="39"/>
-        <item x="9"/>
-        <item m="1" x="55"/>
-        <item m="1" x="72"/>
-        <item m="1" x="40"/>
-        <item x="0"/>
-        <item m="1" x="65"/>
-        <item m="1" x="31"/>
+        <item m="1" x="16"/>
         <item x="11"/>
-        <item m="1" x="41"/>
-        <item m="1" x="19"/>
-        <item m="1" x="43"/>
-        <item m="1" x="61"/>
-        <item m="1" x="18"/>
-        <item m="1" x="26"/>
-        <item x="8"/>
-        <item m="1" x="64"/>
-        <item m="1" x="17"/>
-        <item m="1" x="62"/>
-        <item m="1" x="42"/>
-        <item m="1" x="53"/>
-        <item m="1" x="63"/>
-        <item m="1" x="20"/>
-        <item m="1" x="28"/>
-        <item m="1" x="56"/>
-        <item m="1" x="51"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item m="1" x="25"/>
-        <item x="14"/>
-        <item m="1" x="29"/>
-        <item m="1" x="21"/>
-        <item x="16"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1490,113 +1344,70 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="43">
-        <item sd="0" m="1" x="14"/>
-        <item sd="0" m="1" x="24"/>
-        <item sd="0" x="1"/>
-        <item sd="0" m="1" x="39"/>
-        <item sd="0" m="1" x="13"/>
-        <item sd="0" m="1" x="27"/>
-        <item sd="0" x="2"/>
-        <item sd="0" m="1" x="12"/>
-        <item sd="0" m="1" x="23"/>
-        <item sd="0" m="1" x="29"/>
-        <item sd="0" m="1" x="41"/>
-        <item sd="0" m="1" x="35"/>
-        <item sd="0" m="1" x="18"/>
-        <item sd="0" x="4"/>
-        <item sd="0" m="1" x="28"/>
-        <item sd="0" m="1" x="36"/>
-        <item sd="0" m="1" x="38"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="5"/>
-        <item sd="0" m="1" x="22"/>
-        <item sd="0" m="1" x="25"/>
-        <item sd="0" x="8"/>
-        <item sd="0" x="9"/>
-        <item sd="0" m="1" x="32"/>
-        <item sd="0" m="1" x="40"/>
-        <item sd="0" m="1" x="21"/>
-        <item sd="0" x="7"/>
-        <item sd="0" x="3"/>
-        <item sd="0" m="1" x="17"/>
-        <item sd="0" m="1" x="30"/>
-        <item sd="0" x="0"/>
-        <item sd="0" m="1" x="37"/>
-        <item sd="0" m="1" x="16"/>
-        <item sd="0" x="10"/>
-        <item sd="0" m="1" x="26"/>
-        <item sd="0" m="1" x="19"/>
-        <item sd="0" m="1" x="15"/>
-        <item sd="0" m="1" x="34"/>
-        <item sd="0" m="1" x="31"/>
-        <item sd="0" m="1" x="20"/>
-        <item sd="0" m="1" x="33"/>
-        <item x="11"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="4">
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="37">
+    <pivotField axis="axisCol" showAll="0">
+      <items count="43">
+        <item sd="0" m="1" x="11"/>
+        <item sd="0" m="1" x="22"/>
+        <item sd="0" m="1" x="8"/>
+        <item sd="0" m="1" x="39"/>
+        <item sd="0" m="1" x="10"/>
+        <item sd="0" m="1" x="25"/>
+        <item sd="0" x="1"/>
+        <item sd="0" m="1" x="9"/>
+        <item sd="0" m="1" x="21"/>
+        <item sd="0" m="1" x="27"/>
+        <item sd="0" m="1" x="41"/>
+        <item sd="0" m="1" x="34"/>
+        <item sd="0" m="1" x="16"/>
+        <item x="2"/>
+        <item sd="0" m="1" x="26"/>
+        <item sd="0" m="1" x="35"/>
+        <item sd="0" m="1" x="38"/>
+        <item x="4"/>
+        <item sd="0" m="1" x="30"/>
+        <item sd="0" m="1" x="20"/>
+        <item sd="0" m="1" x="23"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" m="1" x="31"/>
+        <item sd="0" m="1" x="40"/>
+        <item sd="0" m="1" x="19"/>
+        <item sd="0" m="1" x="36"/>
+        <item sd="0" x="3"/>
+        <item sd="0" m="1" x="15"/>
+        <item sd="0" m="1" x="28"/>
+        <item sd="0" x="0"/>
+        <item sd="0" m="1" x="37"/>
+        <item sd="0" m="1" x="14"/>
+        <item sd="0" m="1" x="12"/>
+        <item sd="0" m="1" x="24"/>
+        <item sd="0" m="1" x="17"/>
         <item sd="0" m="1" x="13"/>
-        <item sd="0" m="1" x="9"/>
-        <item sd="0" m="1" x="31"/>
         <item sd="0" m="1" x="33"/>
-        <item sd="0" x="2"/>
-        <item sd="0" m="1" x="7"/>
         <item sd="0" m="1" x="29"/>
         <item sd="0" m="1" x="18"/>
-        <item sd="0" m="1" x="26"/>
-        <item sd="0" m="1" x="30"/>
-        <item sd="0" m="1" x="22"/>
-        <item sd="0" m="1" x="21"/>
-        <item sd="0" m="1" x="12"/>
-        <item sd="0" m="1" x="14"/>
-        <item sd="0" m="1" x="16"/>
-        <item sd="0" m="1" x="6"/>
-        <item sd="0" m="1" x="35"/>
-        <item sd="0" m="1" x="23"/>
         <item sd="0" m="1" x="32"/>
-        <item sd="0" m="1" x="11"/>
-        <item sd="0" m="1" x="28"/>
-        <item sd="0" m="1" x="27"/>
-        <item sd="0" m="1" x="34"/>
-        <item sd="0" m="1" x="19"/>
-        <item sd="0" x="1"/>
-        <item sd="0" m="1" x="17"/>
-        <item sd="0" m="1" x="4"/>
-        <item sd="0" x="0"/>
-        <item sd="0" m="1" x="15"/>
-        <item sd="0" m="1" x="8"/>
-        <item sd="0" m="1" x="5"/>
-        <item sd="0" m="1" x="25"/>
-        <item sd="0" m="1" x="20"/>
-        <item sd="0" m="1" x="10"/>
-        <item sd="0" m="1" x="24"/>
-        <item x="3"/>
+        <item x="7"/>
         <item t="default"/>
       </items>
     </pivotField>
   </pivotFields>
-  <rowFields count="2">
-    <field x="16"/>
+  <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="3">
     <i>
-      <x v="4"/>
+      <x v="33"/>
     </i>
     <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="35"/>
-    </i>
-    <i r="1">
       <x v="56"/>
     </i>
     <i t="grand">
@@ -1604,42 +1415,38 @@
     </i>
   </rowItems>
   <colFields count="2">
-    <field x="15"/>
+    <field x="16"/>
     <field x="1"/>
   </colFields>
-  <colItems count="14">
-    <i>
-      <x v="2"/>
-    </i>
+  <colItems count="12">
     <i>
       <x v="6"/>
     </i>
     <i>
       <x v="13"/>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x v="49"/>
+    </i>
+    <i t="default">
+      <x v="13"/>
     </i>
     <i>
       <x v="17"/>
+      <x v="56"/>
     </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="26"/>
+    <i t="default">
+      <x v="17"/>
     </i>
     <i>
       <x v="27"/>
     </i>
     <i>
       <x v="30"/>
-    </i>
-    <i>
-      <x v="33"/>
     </i>
     <i>
       <x v="41"/>
@@ -1652,6 +1459,9 @@
       <x/>
     </i>
   </colItems>
+  <pageFields count="1">
+    <pageField fld="15" hier="-1"/>
+  </pageFields>
   <dataFields count="1">
     <dataField name="Count of RHS" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
@@ -1964,15 +1774,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1983,7 +1793,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -1992,40 +1802,43 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="H1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
       <c r="L1" t="s">
         <v>8</v>
       </c>
       <c r="M1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="N1" t="s">
         <v>9</v>
       </c>
       <c r="O1" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -2033,7 +1846,7 @@
         <v>14</v>
       </c>
       <c r="D2">
-        <v>1.0828462003628301</v>
+        <v>102</v>
       </c>
       <c r="E2">
         <v>0.645569620253165</v>
@@ -2045,408 +1858,432 @@
         <v>0.778481012658228</v>
       </c>
       <c r="H2">
-        <v>102</v>
+        <v>1.0828462003628301</v>
       </c>
       <c r="I2">
+        <v>6.3445507872800205E-2</v>
+      </c>
+      <c r="J2">
+        <v>0.28067379922604102</v>
+      </c>
+      <c r="K2">
         <v>4.0902255639097698</v>
-      </c>
-      <c r="J2">
-        <v>6.3445507872800205E-2</v>
-      </c>
-      <c r="K2">
-        <v>9.1000000000000004E-3</v>
       </c>
       <c r="L2">
         <v>1.81198382412186</v>
       </c>
       <c r="M2">
-        <v>0.28067379922604102</v>
+        <v>9.2329439926258097</v>
       </c>
       <c r="N2">
         <v>7.7238946177791404E-4</v>
       </c>
       <c r="O2">
-        <v>3</v>
-      </c>
-      <c r="P2" t="s">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+      <c r="Q2" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3">
-        <v>1.12143898881867</v>
+        <v>80</v>
       </c>
       <c r="E3">
-        <v>0.462025316455696</v>
+        <v>0.506329113924051</v>
       </c>
       <c r="F3">
-        <v>0.85882352941176499</v>
+        <v>0.85106382978723405</v>
       </c>
       <c r="G3">
-        <v>0.537974683544304</v>
+        <v>0.59493670886076</v>
       </c>
       <c r="H3">
-        <v>73</v>
+        <v>1.1113064884824999</v>
       </c>
       <c r="I3">
-        <v>3.1684027777777799</v>
+        <v>8.5241044977107494E-2</v>
       </c>
       <c r="J3">
-        <v>9.3000744601638097E-2</v>
+        <v>0.225628230261985</v>
       </c>
       <c r="K3">
-        <v>1.32E-2</v>
+        <v>3.2055749128919899</v>
       </c>
       <c r="L3">
-        <v>1.45422802106559</v>
+        <v>1.4936951655941699</v>
       </c>
       <c r="M3">
-        <v>0.208549006511939</v>
+        <v>6.8793892882922503</v>
       </c>
       <c r="N3">
-        <v>2.56285631828944E-3</v>
+        <v>2.1365073142274099E-3</v>
       </c>
       <c r="O3">
-        <v>3</v>
-      </c>
-      <c r="P3" t="s">
-        <v>23</v>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
       </c>
       <c r="Q3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4">
-        <v>1.1113064884824999</v>
+        <v>99</v>
       </c>
       <c r="E4">
-        <v>0.506329113924051</v>
+        <v>0.626582278481013</v>
       </c>
       <c r="F4">
-        <v>0.85106382978723405</v>
+        <v>0.83193277310924396</v>
       </c>
       <c r="G4">
-        <v>0.59493670886076</v>
+        <v>0.753164556962025</v>
       </c>
       <c r="H4">
-        <v>80</v>
+        <v>1.08632543926662</v>
       </c>
       <c r="I4">
-        <v>3.2055749128919899</v>
+        <v>6.6109988299117198E-2</v>
       </c>
       <c r="J4">
-        <v>8.5241044977107494E-2</v>
+        <v>0.272527954395966</v>
       </c>
       <c r="K4">
-        <v>1.32E-2</v>
+        <v>3.8250000000000002</v>
       </c>
       <c r="L4">
-        <v>1.4936951655941699</v>
+        <v>1.72789193530244</v>
       </c>
       <c r="M4">
-        <v>0.225628230261985</v>
+        <v>8.4673263999227899</v>
       </c>
       <c r="N4">
-        <v>2.1365073142274099E-3</v>
+        <v>9.8327872889956893E-4</v>
       </c>
       <c r="O4">
-        <v>3</v>
-      </c>
-      <c r="P4" t="s">
-        <v>13</v>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
       </c>
       <c r="Q4" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5">
-        <v>1.09211119459053</v>
+        <v>67</v>
       </c>
       <c r="E5">
-        <v>0.582278481012658</v>
+        <v>0.424050632911392</v>
       </c>
       <c r="F5">
-        <v>0.83636363636363598</v>
+        <v>0.88157894736842102</v>
       </c>
       <c r="G5">
-        <v>0.69620253164557</v>
+        <v>0.481012658227848</v>
       </c>
       <c r="H5">
-        <v>92</v>
+        <v>1.1511526750761201</v>
       </c>
       <c r="I5">
-        <v>3.3486590038314201</v>
+        <v>0.115756162558294</v>
       </c>
       <c r="J5">
-        <v>7.0540851553509795E-2</v>
+        <v>0.21831317732055899</v>
       </c>
       <c r="K5">
-        <v>1.32E-2</v>
+        <v>3.8600823045267498</v>
       </c>
       <c r="L5">
-        <v>1.5535635949761399</v>
+        <v>1.6795218483229</v>
       </c>
       <c r="M5">
-        <v>0.24822838631301899</v>
+        <v>8.8717127512210006</v>
       </c>
       <c r="N5">
-        <v>1.8891248571212499E-3</v>
+        <v>7.5582914448785198E-4</v>
       </c>
       <c r="O5">
-        <v>3</v>
-      </c>
-      <c r="P5" t="s">
-        <v>29</v>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
       </c>
       <c r="Q5" t="s">
         <v>17</v>
       </c>
+      <c r="R5" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6">
-        <v>1.1511526750761201</v>
+        <v>93</v>
       </c>
       <c r="E6">
-        <v>0.424050632911392</v>
+        <v>0.588607594936709</v>
       </c>
       <c r="F6">
-        <v>0.88157894736842102</v>
+        <v>0.83035714285714302</v>
       </c>
       <c r="G6">
-        <v>0.481012658227848</v>
+        <v>0.708860759493671</v>
       </c>
       <c r="H6">
-        <v>67</v>
+        <v>1.0842680047225499</v>
       </c>
       <c r="I6">
-        <v>3.8600823045267498</v>
+        <v>6.4534358047016294E-2</v>
       </c>
       <c r="J6">
-        <v>0.115756162558294</v>
+        <v>0.235221421215242</v>
       </c>
       <c r="K6">
-        <v>9.1000000000000004E-3</v>
+        <v>3.1466165413533802</v>
       </c>
       <c r="L6">
-        <v>1.6795218483229</v>
+        <v>1.45577217627033</v>
       </c>
       <c r="M6">
-        <v>0.21831317732055899</v>
+        <v>6.8013359643165403</v>
       </c>
       <c r="N6">
-        <v>7.5582914448785198E-4</v>
+        <v>3.3158310083905101E-3</v>
       </c>
       <c r="O6">
-        <v>3</v>
-      </c>
-      <c r="P6" t="s">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>26</v>
+      </c>
+      <c r="R6" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7">
-        <v>1.0842680047225499</v>
+        <v>93</v>
       </c>
       <c r="E7">
         <v>0.588607594936709</v>
       </c>
       <c r="F7">
-        <v>0.83035714285714302</v>
+        <v>0.83783783783783805</v>
       </c>
       <c r="G7">
-        <v>0.708860759493671</v>
+        <v>0.70253164556962</v>
       </c>
       <c r="H7">
-        <v>93</v>
+        <v>1.09403618494528</v>
       </c>
       <c r="I7">
-        <v>3.1466165413533802</v>
+        <v>7.2015053027711301E-2</v>
       </c>
       <c r="J7">
-        <v>6.4534358047016294E-2</v>
+        <v>0.25791300796406003</v>
       </c>
       <c r="K7">
-        <v>1.32E-2</v>
+        <v>3.50595238095238</v>
       </c>
       <c r="L7">
-        <v>1.45577217627033</v>
+        <v>1.6220177643011999</v>
       </c>
       <c r="M7">
-        <v>0.235221421215242</v>
+        <v>7.5780317380193498</v>
       </c>
       <c r="N7">
-        <v>3.3158310083905101E-3</v>
+        <v>1.3413825557096299E-3</v>
       </c>
       <c r="O7">
-        <v>3</v>
-      </c>
-      <c r="P7" t="s">
-        <v>29</v>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="P7">
+        <v>2</v>
       </c>
       <c r="Q7" t="s">
+        <v>22</v>
+      </c>
+      <c r="R7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8">
-        <v>1.08632543926662</v>
+        <v>92</v>
       </c>
       <c r="E8">
-        <v>0.626582278481013</v>
+        <v>0.582278481012658</v>
       </c>
       <c r="F8">
-        <v>0.83193277310924396</v>
+        <v>0.83636363636363598</v>
       </c>
       <c r="G8">
-        <v>0.753164556962025</v>
+        <v>0.69620253164557</v>
       </c>
       <c r="H8">
-        <v>99</v>
+        <v>1.09211119459053</v>
       </c>
       <c r="I8">
-        <v>3.8250000000000002</v>
+        <v>7.0540851553509795E-2</v>
       </c>
       <c r="J8">
-        <v>6.6109988299117198E-2</v>
+        <v>0.24822838631301899</v>
       </c>
       <c r="K8">
-        <v>9.1000000000000004E-3</v>
+        <v>3.3486590038314201</v>
       </c>
       <c r="L8">
-        <v>1.72789193530244</v>
+        <v>1.5535635949761399</v>
       </c>
       <c r="M8">
-        <v>0.272527954395966</v>
+        <v>7.21793247486172</v>
       </c>
       <c r="N8">
-        <v>9.8327872889956893E-4</v>
+        <v>1.8891248571212499E-3</v>
       </c>
       <c r="O8">
-        <v>3</v>
-      </c>
-      <c r="P8" t="s">
-        <v>25</v>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="P8">
+        <v>2</v>
       </c>
       <c r="Q8" t="s">
+        <v>26</v>
+      </c>
+      <c r="R8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9">
-        <v>1.1070786920589299</v>
+        <v>97</v>
       </c>
       <c r="E9">
-        <v>0.493670886075949</v>
+        <v>0.613924050632911</v>
       </c>
       <c r="F9">
-        <v>0.84782608695652195</v>
+        <v>0.83620689655172398</v>
       </c>
       <c r="G9">
-        <v>0.582278481012658</v>
+        <v>0.734177215189874</v>
       </c>
       <c r="H9">
-        <v>78</v>
+        <v>1.0919065260758001</v>
       </c>
       <c r="I9">
-        <v>2.9800664451827199</v>
+        <v>7.0384111741597505E-2</v>
       </c>
       <c r="J9">
-        <v>8.2003302146395202E-2</v>
+        <v>0.27522935779816499</v>
       </c>
       <c r="K9">
-        <v>1.32E-2</v>
+        <v>3.82894736842105</v>
       </c>
       <c r="L9">
-        <v>1.3914650555213</v>
+        <v>1.74750749450523</v>
       </c>
       <c r="M9">
-        <v>0.209306409130816</v>
+        <v>8.3895708580576898</v>
       </c>
       <c r="N9">
-        <v>3.7727982342369501E-3</v>
+        <v>8.0570904900294997E-4</v>
       </c>
       <c r="O9">
-        <v>3</v>
-      </c>
-      <c r="P9" t="s">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="P9">
+        <v>2</v>
+      </c>
+      <c r="Q9" t="s">
         <v>22</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -2457,7 +2294,7 @@
         <v>14</v>
       </c>
       <c r="D10">
-        <v>1.1251978195885399</v>
+        <v>81</v>
       </c>
       <c r="E10">
         <v>0.512658227848101</v>
@@ -2469,405 +2306,149 @@
         <v>0.594936708860759</v>
       </c>
       <c r="H10">
-        <v>81</v>
+        <v>1.1251978195885399</v>
       </c>
       <c r="I10">
+        <v>9.5879342849447893E-2</v>
+      </c>
+      <c r="J10">
+        <v>0.25378720370700403</v>
+      </c>
+      <c r="K10">
         <v>3.7384615384615398</v>
-      </c>
-      <c r="J10">
-        <v>9.5879342849447893E-2</v>
-      </c>
-      <c r="K10">
-        <v>7.7999999999999996E-3</v>
       </c>
       <c r="L10">
         <v>1.7240849535192999</v>
       </c>
       <c r="M10">
-        <v>0.25378720370700403</v>
+        <v>8.1063839957697095</v>
       </c>
       <c r="N10">
         <v>5.9937858995312804E-4</v>
       </c>
       <c r="O10">
-        <v>3</v>
-      </c>
-      <c r="P10" t="s">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="P10">
+        <v>2</v>
+      </c>
+      <c r="Q10" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11">
-        <v>1.1284562799714299</v>
+        <v>61</v>
       </c>
       <c r="E11">
-        <v>0.443037974683544</v>
+        <v>0.386075949367089</v>
       </c>
       <c r="F11">
-        <v>0.86419753086419704</v>
+        <v>0.89705882352941202</v>
       </c>
       <c r="G11">
-        <v>0.512658227848101</v>
+        <v>0.430379746835443</v>
       </c>
       <c r="H11">
-        <v>70</v>
+        <v>1.17136606708799</v>
       </c>
       <c r="I11">
-        <v>3.24420677361854</v>
+        <v>0.13123603871928499</v>
       </c>
       <c r="J11">
-        <v>9.83747460540709E-2</v>
+        <v>0.210353573027003</v>
       </c>
       <c r="K11">
-        <v>1.32E-2</v>
+        <v>4.3571428571428603</v>
       </c>
       <c r="L11">
-        <v>1.4694879318405401</v>
+        <v>1.77754958841213</v>
       </c>
       <c r="M11">
-        <v>0.20448270261491</v>
+        <v>10.680261187261699</v>
       </c>
       <c r="N11">
-        <v>2.3400287404868598E-3</v>
+        <v>4.9535558537442802E-4</v>
       </c>
       <c r="O11">
-        <v>3</v>
-      </c>
-      <c r="P11" t="s">
-        <v>35</v>
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
       </c>
       <c r="Q11" t="s">
+        <v>24</v>
+      </c>
+      <c r="R11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12">
-        <v>1.09403618494528</v>
+        <v>61</v>
       </c>
       <c r="E12">
-        <v>0.588607594936709</v>
+        <v>0.386075949367089</v>
       </c>
       <c r="F12">
-        <v>0.83783783783783805</v>
+        <v>0.89705882352941202</v>
       </c>
       <c r="G12">
-        <v>0.70253164556962</v>
+        <v>0.430379746835443</v>
       </c>
       <c r="H12">
-        <v>93</v>
+        <v>1.17136606708799</v>
       </c>
       <c r="I12">
-        <v>3.50595238095238</v>
+        <v>0.13123603871928499</v>
       </c>
       <c r="J12">
-        <v>7.2015053027711301E-2</v>
+        <v>0.210353573027003</v>
       </c>
       <c r="K12">
-        <v>1.0699999999999999E-2</v>
+        <v>4.3571428571428603</v>
       </c>
       <c r="L12">
-        <v>1.6220177643011999</v>
+        <v>1.77754958841213</v>
       </c>
       <c r="M12">
-        <v>0.25791300796406003</v>
+        <v>10.680261187261699</v>
       </c>
       <c r="N12">
-        <v>1.3413825557096299E-3</v>
+        <v>4.9535558537442802E-4</v>
       </c>
       <c r="O12">
-        <v>3</v>
-      </c>
-      <c r="P12" t="s">
-        <v>25</v>
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
       </c>
       <c r="Q12" t="s">
+        <v>23</v>
+      </c>
+      <c r="R12" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13">
-        <v>1.0919065260758001</v>
-      </c>
-      <c r="E13">
-        <v>0.613924050632911</v>
-      </c>
-      <c r="F13">
-        <v>0.83620689655172398</v>
-      </c>
-      <c r="G13">
-        <v>0.734177215189874</v>
-      </c>
-      <c r="H13">
-        <v>97</v>
-      </c>
-      <c r="I13">
-        <v>3.82894736842105</v>
-      </c>
-      <c r="J13">
-        <v>7.0384111741597505E-2</v>
-      </c>
-      <c r="K13">
-        <v>9.1000000000000004E-3</v>
-      </c>
-      <c r="L13">
-        <v>1.74750749450523</v>
-      </c>
-      <c r="M13">
-        <v>0.27522935779816499</v>
-      </c>
-      <c r="N13">
-        <v>8.0570904900294997E-4</v>
-      </c>
-      <c r="O13">
-        <v>3</v>
-      </c>
-      <c r="P13" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14">
-        <v>1.17136606708799</v>
-      </c>
-      <c r="E14">
-        <v>0.386075949367089</v>
-      </c>
-      <c r="F14">
-        <v>0.89705882352941202</v>
-      </c>
-      <c r="G14">
-        <v>0.430379746835443</v>
-      </c>
-      <c r="H14">
-        <v>61</v>
-      </c>
-      <c r="I14">
-        <v>4.3571428571428603</v>
-      </c>
-      <c r="J14">
-        <v>0.13123603871928499</v>
-      </c>
-      <c r="K14">
-        <v>7.4000000000000003E-3</v>
-      </c>
-      <c r="L14">
-        <v>1.77754958841213</v>
-      </c>
-      <c r="M14">
-        <v>0.210353573027003</v>
-      </c>
-      <c r="N14">
-        <v>4.9535558537442802E-4</v>
-      </c>
-      <c r="O14">
-        <v>2</v>
-      </c>
-      <c r="P14" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15">
-        <v>1.17136606708799</v>
-      </c>
-      <c r="E15">
-        <v>0.386075949367089</v>
-      </c>
-      <c r="F15">
-        <v>0.89705882352941202</v>
-      </c>
-      <c r="G15">
-        <v>0.430379746835443</v>
-      </c>
-      <c r="H15">
-        <v>61</v>
-      </c>
-      <c r="I15">
-        <v>4.3571428571428603</v>
-      </c>
-      <c r="J15">
-        <v>0.13123603871928499</v>
-      </c>
-      <c r="K15">
-        <v>7.4000000000000003E-3</v>
-      </c>
-      <c r="L15">
-        <v>1.77754958841213</v>
-      </c>
-      <c r="M15">
-        <v>0.210353573027003</v>
-      </c>
-      <c r="N15">
-        <v>4.9535558537442802E-4</v>
-      </c>
-      <c r="O15">
-        <v>2</v>
-      </c>
-      <c r="P15" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16">
-        <v>1.0996085254458501</v>
-      </c>
-      <c r="E16">
-        <v>0.506329113924051</v>
-      </c>
-      <c r="F16">
-        <v>0.84210526315789502</v>
-      </c>
-      <c r="G16">
-        <v>0.60126582278481</v>
-      </c>
-      <c r="H16">
-        <v>80</v>
-      </c>
-      <c r="I16">
-        <v>2.8617886178861802</v>
-      </c>
-      <c r="J16">
-        <v>7.6282478347768107E-2</v>
-      </c>
-      <c r="K16">
-        <v>1.32E-2</v>
-      </c>
-      <c r="L16">
-        <v>1.34292165572156</v>
-      </c>
-      <c r="M16">
-        <v>0.205602442090142</v>
-      </c>
-      <c r="N16">
-        <v>5.0826707024197396E-3</v>
-      </c>
-      <c r="O16">
-        <v>3</v>
-      </c>
-      <c r="P16" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17">
-        <v>1.19875355642867</v>
-      </c>
-      <c r="E17">
-        <v>0.354430379746835</v>
-      </c>
-      <c r="F17">
-        <v>0.91803278688524603</v>
-      </c>
-      <c r="G17">
-        <v>0.386075949367089</v>
-      </c>
-      <c r="H17">
-        <v>56</v>
-      </c>
-      <c r="I17">
-        <v>5.5138461538461501</v>
-      </c>
-      <c r="J17">
-        <v>0.15221000207511901</v>
-      </c>
-      <c r="K17">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="L17">
-        <v>2.0122604092032601</v>
-      </c>
-      <c r="M17">
-        <v>0.20966128340717399</v>
-      </c>
-      <c r="N17">
-        <v>1.8980410385483401E-4</v>
-      </c>
-      <c r="O17">
-        <v>1</v>
-      </c>
-      <c r="P17" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2877,33 +2458,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:O11"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="8.5" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="14.5" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7.33203125" bestFit="1" customWidth="1"/>
@@ -2974,234 +2557,167 @@
     <col min="105" max="117" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" t="s">
-        <v>43</v>
-      </c>
-      <c r="O4" t="s">
-        <v>41</v>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
       <c r="F6" s="1">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1">
+      <c r="M6" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1">
         <v>1</v>
       </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
         <v>3</v>
       </c>
-      <c r="E7" s="1">
+      <c r="G8" s="1">
         <v>1</v>
       </c>
-      <c r="F7" s="1">
+      <c r="H8" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1">
+      <c r="I8" s="1">
         <v>2</v>
       </c>
-      <c r="K7" s="1">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1">
-        <v>1</v>
-      </c>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1">
-        <v>1</v>
-      </c>
+      <c r="J8" s="1">
+        <v>2</v>
+      </c>
+      <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>3</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="I11" s="1">
-        <v>1</v>
-      </c>
-      <c r="J11" s="1">
-        <v>2</v>
-      </c>
-      <c r="K11" s="1">
-        <v>2</v>
-      </c>
-      <c r="L11" s="1">
-        <v>1</v>
-      </c>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1">
-        <v>16</v>
+      <c r="M8" s="1">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>